<commit_message>
#12238 feedback to remove mumbai district, sum of % and alphabetic order
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12238 Vitamin K Performance/50. Vitamin K performance report.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12238 Vitamin K Performance/50. Vitamin K performance report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="23895" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
   <si>
     <t>State Family Welfare Bureau,Pune</t>
   </si>
@@ -143,7 +143,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +184,152 @@
       <name val="Verdana"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,7 +338,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79995117038483843"/>
+        <fgColor theme="3" tint="0.799951170384838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -198,8 +348,194 @@
         <bgColor rgb="FFCCFF99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -296,28 +632,297 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -327,44 +932,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -626,293 +1248,293 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.85714285714286" customWidth="1"/>
+    <col min="2" max="2" width="11.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="17.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="18.5714285714286" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5714285714286" customWidth="1"/>
+    <col min="9" max="9" width="21.7142857142857" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
-    <col min="13" max="14" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.7142857142857" customWidth="1"/>
+    <col min="12" max="12" width="18.5714285714286" customWidth="1"/>
+    <col min="13" max="14" width="18.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" ht="17.25" spans="1:14">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="10"/>
-    </row>
-    <row r="2" spans="1:14" ht="17.25">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="17"/>
+    </row>
+    <row r="2" ht="17.25" spans="1:14">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="13"/>
-    </row>
-    <row r="3" spans="1:14" ht="17.25">
-      <c r="A3" s="15" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" ht="17.25" spans="1:14">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="11" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="13"/>
-    </row>
-    <row r="4" spans="1:14" ht="17.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14" t="s">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" ht="17.25" spans="1:14">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="9"/>
+      <c r="K4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="14"/>
-    </row>
-    <row r="5" spans="1:14" ht="48" customHeight="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="2" t="s">
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" ht="48" customHeight="1" spans="1:14">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="60">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+    <row r="6" s="1" customFormat="1" ht="60" spans="1:14">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="33.75">
-      <c r="E8" s="5" t="s">
+    <row r="8" ht="33.75" spans="5:5">
+      <c r="E8" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="E9" s="6" t="s">
+    <row r="9" spans="5:5">
+      <c r="E9" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="E10" s="6" t="s">
+    <row r="10" spans="5:5">
+      <c r="E10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="E11" s="6" t="s">
+    <row r="11" spans="5:5">
+      <c r="E11" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="E12" s="6" t="s">
+    <row r="12" spans="5:5">
+      <c r="E12" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="E13" s="6" t="s">
+    <row r="13" spans="5:5">
+      <c r="E13" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="E14" s="6" t="s">
+    <row r="14" spans="5:5">
+      <c r="E14" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="E15" s="6" t="s">
+    <row r="15" spans="5:5">
+      <c r="E15" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="E16" s="6" t="s">
+    <row r="16" spans="5:5">
+      <c r="E16" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="5:5">
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="5:5">
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="5:5">
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="5:5">
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="5:5" ht="45">
-      <c r="E21" s="5" t="s">
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" ht="45" spans="5:5">
+      <c r="E21" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="5:5">
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="5:5">
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="5:5">
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="5:5">
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="26" spans="5:5">
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -931,7 +1553,8 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>